<commit_message>
work on electronic package
</commit_message>
<xml_diff>
--- a/inst/templates/DataImportConfiguration.xlsx
+++ b/inst/templates/DataImportConfiguration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataFiles" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
   <si>
     <t xml:space="preserve">FileIdentifier</t>
   </si>
@@ -307,127 +307,130 @@
     <t xml:space="preserve">year(s)</t>
   </si>
   <si>
+    <t xml:space="preserve">optional,  please provide source unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGHT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HGHT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use characters Male Female (case insensitive) or numeric coding  1=male 2= female </t>
+  </si>
+  <si>
+    <t xml:space="preserve">population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RACENAME == "White"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"European_ICRP_2002"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character, PK Sim population name (get available list by calling ospsuite::HumanPopulation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RACENAME == "Asian"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Asian_Tanaka_1996"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Human"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character, PK-Sim Species name (ospsuite::Species)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covariate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNTRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example for covariate, please delete if not used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta data used for PK-Sim import, if not available, delete row or set all values to NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pkParameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parameter name as defined in PKParameter.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">errorType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"GeometricStdDev"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errorValues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ignored for individual data </t>
+  </si>
+  <si>
     <t xml:space="preserve">character, age BI</t>
   </si>
   <si>
-    <t xml:space="preserve">weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WGHT0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg</t>
-  </si>
-  <si>
     <t xml:space="preserve">character, weight BI</t>
   </si>
   <si>
-    <t xml:space="preserve">height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HGHT0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm</t>
-  </si>
-  <si>
     <t xml:space="preserve">character, height BI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use characters Male Female (case insensitive) or numeric coding  1=male 2= female </t>
-  </si>
-  <si>
-    <t xml:space="preserve">population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RACENAME == "White"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"European_ICRP_2002"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character, PK Sim population name (get available list by calling ospsuite::HumanPopulation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RACENAME == "Asian"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Asian_Tanaka_1996"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Human"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character, PK-Sim Species name (ospsuite::Species)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">covariate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">example for covariate, please delete if not used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meta data used for PK-Sim import, if not available, delete row or set all values to NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">route</t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pkParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parameter name as defined in PKParameter.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">errorType </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"GeometricStdDev"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errorValues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ignored for individual data </t>
   </si>
 </sst>
 </file>
@@ -852,13 +855,13 @@
   </sheetPr>
   <dimension ref="A1:F1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.84"/>
@@ -902,7 +905,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3942,8 +3945,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4273,77 +4276,77 @@
         <v>82</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G21" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>76</v>
@@ -4353,29 +4356,29 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="G26" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>32</v>
@@ -4387,12 +4390,12 @@
         <v>69</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>32</v>
@@ -4404,12 +4407,12 @@
         <v>69</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>32</v>
@@ -4421,12 +4424,12 @@
         <v>69</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>32</v>
@@ -4438,12 +4441,12 @@
         <v>69</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>32</v>
@@ -4455,7 +4458,7 @@
         <v>69</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4641,21 +4644,21 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
@@ -4666,10 +4669,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>57</v>
@@ -4680,16 +4683,16 @@
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>64</v>
@@ -4697,10 +4700,10 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>66</v>
@@ -4711,10 +4714,10 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>39</v>
@@ -4728,10 +4731,10 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>39</v>
@@ -4748,7 +4751,7 @@
         <v>72</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>39</v>
@@ -4757,7 +4760,7 @@
         <v>69</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4774,7 +4777,7 @@
         <v>78</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4791,77 +4794,77 @@
         <v>82</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G19" s="9" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>76</v>
@@ -4871,29 +4874,29 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="G24" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>32</v>
@@ -4905,12 +4908,12 @@
         <v>69</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>32</v>
@@ -4922,12 +4925,12 @@
         <v>69</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>32</v>
@@ -4939,12 +4942,12 @@
         <v>69</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>32</v>
@@ -4956,12 +4959,12 @@
         <v>69</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>32</v>
@@ -4973,7 +4976,7 @@
         <v>69</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>